<commit_message>
add ttest and requirements.txt
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
@@ -564,6 +564,40 @@
   <si>
     <t xml:space="preserve">Class, which does segmentation by threshold value</t>
   </si>
+  <si>
+    <t xml:space="preserve">get_ttest_p_value_df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform the independent t-test test on two groups.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hyper_imges: tp.Sequence[HyperImg],            
+target_variable_1: str, 
+target_variable_2: str,  
+alternative: str = 'two-sided',
+params_scipy: dict[str, tp.Any] | None = None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pd.DataFrame: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_ttest_p_value_graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plots p-value of independent t-test criterion versus wavelength.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hyper_imges: tp.Sequence[HyperImg], 
+target_variable_1: str,                            
+target_variable_2: str,                             
+alternative: str = 'two-sided',                             
+params_scipy: dict[str, tp.Any] | None = None,                             
+download_path: str = '',                             
+with_png: bool = False,                             
+png_scale: float = 8,                             
+png_width: int = 500,                             
+Png_height: int = 700</t>
+  </si>
 </sst>
 </file>
 
@@ -572,11 +606,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -596,6 +631,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -648,7 +689,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -663,6 +704,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -742,13 +787,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.64"/>
@@ -1406,6 +1451,47 @@
         <v>125</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">-D36</f>
+        <v>-0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>